<commit_message>
Just realized I made a huge mistake in HW3. Fixed it now.
</commit_message>
<xml_diff>
--- a/Build/Code/example_presentation/capital_data.xlsx
+++ b/Build/Code/example_presentation/capital_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\projects\ECON691ER\Build\Code\example_presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64900A0D-DF0D-4568-90F8-2F3AEFF34611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64ED331-94FD-49C3-B042-0B118D4F79C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95471448-2463-426F-8CAE-2CE8FB836CEC}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -166,7 +166,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>